<commit_message>
Preenchendo a planilha de análise.
</commit_message>
<xml_diff>
--- a/AlgoritmosDeOrdenacao/Análise dos algoritmos.xlsx
+++ b/AlgoritmosDeOrdenacao/Análise dos algoritmos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" tabRatio="854"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" tabRatio="854" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Aleatórios Distintos" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>Aleatório Distintos</t>
   </si>
@@ -71,6 +71,129 @@
   </si>
   <si>
     <t>Decrescentes Repetidos</t>
+  </si>
+  <si>
+    <t>10.67</t>
+  </si>
+  <si>
+    <t>23.0</t>
+  </si>
+  <si>
+    <t>29.0</t>
+  </si>
+  <si>
+    <t>43.33</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>58.0</t>
+  </si>
+  <si>
+    <t>65.67</t>
+  </si>
+  <si>
+    <t>83.0</t>
+  </si>
+  <si>
+    <t>82.33</t>
+  </si>
+  <si>
+    <t>98.0</t>
+  </si>
+  <si>
+    <t>103.67</t>
+  </si>
+  <si>
+    <t>4.33</t>
+  </si>
+  <si>
+    <t>11.33</t>
+  </si>
+  <si>
+    <t>15.0</t>
+  </si>
+  <si>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t>18.67</t>
+  </si>
+  <si>
+    <t>26.33</t>
+  </si>
+  <si>
+    <t>29.67</t>
+  </si>
+  <si>
+    <t>31.0</t>
+  </si>
+  <si>
+    <t>32.0</t>
+  </si>
+  <si>
+    <t>6.83</t>
+  </si>
+  <si>
+    <t>14.17</t>
+  </si>
+  <si>
+    <t>14.83</t>
+  </si>
+  <si>
+    <t>19.0</t>
+  </si>
+  <si>
+    <t>28.33</t>
+  </si>
+  <si>
+    <t>28.17</t>
+  </si>
+  <si>
+    <t>33.67</t>
+  </si>
+  <si>
+    <t>44.0</t>
+  </si>
+  <si>
+    <t>45.5</t>
+  </si>
+  <si>
+    <t>99.67</t>
+  </si>
+  <si>
+    <t>49.17</t>
+  </si>
+  <si>
+    <t>1.33</t>
+  </si>
+  <si>
+    <t>4.67</t>
+  </si>
+  <si>
+    <t>10.33</t>
+  </si>
+  <si>
+    <t>13.0</t>
+  </si>
+  <si>
+    <t>22.0</t>
+  </si>
+  <si>
+    <t>24.67</t>
+  </si>
+  <si>
+    <t>25.33</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>27.0</t>
+  </si>
+  <si>
+    <t>31.33</t>
   </si>
 </sst>
 </file>
@@ -284,15 +407,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -344,6 +458,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2462,6 +2585,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1030005263"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3402,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,26 +3542,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -3495,25 +3619,25 @@
       <c r="A5" s="6">
         <v>100000</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>33201.67</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>1291.67</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>5792.33</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <v>20.67</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="12">
         <v>16</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="12">
         <v>21</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -3522,30 +3646,26 @@
         <f>(A5+60000)</f>
         <v>160000</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>62715</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>3656.67</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>10897</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <v>26</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="12">
         <v>15.67</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="12">
         <v>26</v>
       </c>
-      <c r="H6" s="20">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <f>LARGE(B4:H16,1)</f>
-        <v>1201261</v>
+      <c r="H6" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -3553,25 +3673,25 @@
         <f t="shared" ref="A7:A15" si="0">(A6+60000)</f>
         <v>220000</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="11">
         <v>118385.33</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>6985</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>20010.669999999998</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <v>41.67</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="12">
         <v>31</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="12">
         <v>47</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -3580,25 +3700,25 @@
         <f t="shared" si="0"/>
         <v>280000</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>191690.33</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>11419</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>32675.67</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <v>52.33</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="12">
         <v>36.67</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="12">
         <v>57.33</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="17">
         <v>10.33</v>
       </c>
     </row>
@@ -3607,130 +3727,130 @@
         <f t="shared" si="0"/>
         <v>340000</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>282545.33</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>17199.669999999998</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>48145.67</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <v>62.33</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="12">
         <v>41.33</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="12">
         <v>67.67</v>
       </c>
-      <c r="H9" s="20">
-        <v>0</v>
-      </c>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="18"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
+      <c r="H9" s="17">
+        <v>0</v>
+      </c>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="11">
         <v>391595.67</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>23320.33</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>66663</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <v>78</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="12">
         <v>62.67</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="12">
         <v>78</v>
       </c>
-      <c r="H10" s="20">
-        <v>0</v>
-      </c>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="18"/>
-      <c r="X10" s="18"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
+      <c r="H10" s="17">
+        <v>0</v>
+      </c>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>460000</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>517183.33</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>31367</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>87947.67</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <v>88.33</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="12">
         <v>62.33</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="12">
         <v>94</v>
       </c>
-      <c r="H11" s="20">
-        <v>0</v>
-      </c>
-      <c r="S11" s="17"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="18"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="S11" s="14"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>520000</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="11">
         <v>659194</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>40171</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>112865.33</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <v>93.67</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="12">
         <v>73</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="12">
         <v>109</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="17">
         <v>10.67</v>
       </c>
       <c r="S12" s="9"/>
@@ -3747,185 +3867,185 @@
         <f t="shared" si="0"/>
         <v>580000</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>822865</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>49656.33</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>139525</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="12">
         <v>104</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="12">
         <v>78</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="12">
         <v>125</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="17">
         <v>15</v>
       </c>
-      <c r="S13" s="19"/>
-      <c r="T13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
-      <c r="Z13" s="15"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="12"/>
+      <c r="Z13" s="12"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>640000</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>1002575</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>60709</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>170496.67</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <v>119.67</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="12">
         <v>83.33</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="12">
         <v>130</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="17">
         <v>15.33</v>
       </c>
-      <c r="S14" s="19"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="12"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="13">
         <v>1201261</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="18">
         <v>73111.67</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="18">
         <v>204268.33</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="18">
         <v>130.33000000000001</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="18">
         <v>104.33</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="18">
         <v>172</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="19">
         <v>15.33</v>
       </c>
-      <c r="S15" s="19"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" s="12"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="S16" s="19"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
     </row>
     <row r="17" spans="19:26" x14ac:dyDescent="0.25">
-      <c r="S17" s="19"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
     </row>
     <row r="18" spans="19:26" x14ac:dyDescent="0.25">
-      <c r="S18" s="19"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
     </row>
     <row r="19" spans="19:26" x14ac:dyDescent="0.25">
-      <c r="S19" s="19"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
     </row>
     <row r="20" spans="19:26" x14ac:dyDescent="0.25">
-      <c r="S20" s="19"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
     </row>
     <row r="21" spans="19:26" x14ac:dyDescent="0.25">
-      <c r="S21" s="19"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
     </row>
     <row r="22" spans="19:26" x14ac:dyDescent="0.25">
-      <c r="S22" s="19"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
     </row>
     <row r="23" spans="19:26" x14ac:dyDescent="0.25">
-      <c r="S23" s="19"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="15"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3942,8 +4062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,26 +4072,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -4029,25 +4149,25 @@
       <c r="A5" s="6">
         <v>100000</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>24497.67</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>1406.33</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>4125.33</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <v>15.33</v>
       </c>
-      <c r="F5" s="15">
-        <v>5.33</v>
-      </c>
-      <c r="G5" s="15">
+      <c r="F5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="12">
         <v>21.33</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4056,25 +4176,25 @@
         <f>(A5+60000)</f>
         <v>160000</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>62558</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>3635.67</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>10742</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <v>31</v>
       </c>
-      <c r="F6" s="15">
-        <v>21</v>
-      </c>
-      <c r="G6" s="15">
+      <c r="F6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="12">
         <v>31.33</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4083,25 +4203,25 @@
         <f t="shared" ref="A7:A15" si="0">(A6+60000)</f>
         <v>220000</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="11">
         <v>118549.33</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>7006</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>20325.330000000002</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <v>36.67</v>
       </c>
-      <c r="F7" s="15">
-        <v>31</v>
-      </c>
-      <c r="G7" s="15">
+      <c r="F7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="12">
         <v>47</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4110,25 +4230,25 @@
         <f t="shared" si="0"/>
         <v>280000</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>191932</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>11454.33</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>32878.33</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <v>51.67</v>
       </c>
-      <c r="F8" s="15">
-        <v>36.33</v>
-      </c>
-      <c r="G8" s="15">
+      <c r="F8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="12">
         <v>52.33</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -4137,25 +4257,25 @@
         <f t="shared" si="0"/>
         <v>340000</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>282719.67</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>17231.330000000002</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>48515.67</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <v>62</v>
       </c>
-      <c r="F9" s="15">
-        <v>47</v>
-      </c>
-      <c r="G9" s="15">
+      <c r="F9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="12">
         <v>68.33</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4164,25 +4284,25 @@
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="11">
         <v>391396.67</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>23410</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>66970</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <v>62.67</v>
       </c>
-      <c r="F10" s="15">
-        <v>57.33</v>
-      </c>
-      <c r="G10" s="15">
+      <c r="F10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="12">
         <v>88.67</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4191,25 +4311,25 @@
         <f t="shared" si="0"/>
         <v>460000</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>517556.33</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>31415.33</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>87890.33</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <v>88.67</v>
       </c>
-      <c r="F11" s="15">
-        <v>62.33</v>
-      </c>
-      <c r="G11" s="15">
+      <c r="F11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="12">
         <v>93.67</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="17">
         <v>5</v>
       </c>
     </row>
@@ -4218,25 +4338,25 @@
         <f t="shared" si="0"/>
         <v>520000</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="11">
         <v>661733.32999999996</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>40275.33</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>112762.33</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <v>99</v>
       </c>
-      <c r="F12" s="15">
-        <v>67.67</v>
-      </c>
-      <c r="G12" s="15">
+      <c r="F12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="12">
         <v>109</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="17">
         <v>10.33</v>
       </c>
     </row>
@@ -4245,25 +4365,25 @@
         <f t="shared" si="0"/>
         <v>580000</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>821844.33</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>49890.67</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>140291.32999999999</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="12">
         <v>109.33</v>
       </c>
-      <c r="F13" s="15">
-        <v>78</v>
-      </c>
-      <c r="G13" s="15">
+      <c r="F13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="12">
         <v>125</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="17">
         <v>5</v>
       </c>
     </row>
@@ -4272,25 +4392,25 @@
         <f t="shared" si="0"/>
         <v>640000</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>1001722.33</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>61090</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>171341</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <v>120</v>
       </c>
-      <c r="F14" s="15">
-        <v>88.33</v>
-      </c>
-      <c r="G14" s="15">
+      <c r="F14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="12">
         <v>135.33000000000001</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="17">
         <v>10.67</v>
       </c>
     </row>
@@ -4299,25 +4419,25 @@
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="13">
         <v>1199776.33</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="18">
         <v>73060.33</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="18">
         <v>203748.67</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="18">
         <v>141</v>
       </c>
-      <c r="F15" s="21">
-        <v>88.67</v>
-      </c>
-      <c r="G15" s="21">
+      <c r="F15" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="18">
         <v>156.33000000000001</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="19">
         <v>15.67</v>
       </c>
     </row>
@@ -4335,7 +4455,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H15"/>
+      <selection activeCell="F5" sqref="F5:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4344,50 +4464,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4395,25 +4515,25 @@
       <c r="A4" s="5">
         <v>0</v>
       </c>
-      <c r="B4" s="26">
-        <v>0</v>
-      </c>
-      <c r="C4" s="27">
-        <v>0</v>
-      </c>
-      <c r="D4" s="27">
-        <v>0</v>
-      </c>
-      <c r="E4" s="27">
-        <v>0</v>
-      </c>
-      <c r="F4" s="27">
-        <v>0</v>
-      </c>
-      <c r="G4" s="27">
-        <v>0</v>
-      </c>
-      <c r="H4" s="28">
+      <c r="B4" s="23">
+        <v>0</v>
+      </c>
+      <c r="C4" s="24">
+        <v>0</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0</v>
+      </c>
+      <c r="F4" s="24">
+        <v>0</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0</v>
+      </c>
+      <c r="H4" s="25">
         <v>0</v>
       </c>
     </row>
@@ -4421,23 +4541,25 @@
       <c r="A5" s="6">
         <v>100000</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="26">
         <v>6954</v>
       </c>
-      <c r="C5" s="30">
-        <v>0</v>
-      </c>
-      <c r="D5" s="30">
+      <c r="C5" s="27">
+        <v>0</v>
+      </c>
+      <c r="D5" s="27">
         <v>4119.67</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="27">
         <v>5.33</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30">
+      <c r="F5" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="27">
         <v>10.33</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="29">
         <v>0</v>
       </c>
     </row>
@@ -4446,23 +4568,25 @@
         <f>(A5+60000)</f>
         <v>160000</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="26">
         <v>17944.669999999998</v>
       </c>
-      <c r="C6" s="30">
-        <v>0</v>
-      </c>
-      <c r="D6" s="30">
+      <c r="C6" s="27">
+        <v>0</v>
+      </c>
+      <c r="D6" s="27">
         <v>10590</v>
       </c>
-      <c r="E6" s="30">
-        <v>0</v>
-      </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30">
+      <c r="E6" s="27">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="27">
         <v>15.33</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="29">
         <v>5.33</v>
       </c>
     </row>
@@ -4471,23 +4595,25 @@
         <f t="shared" ref="A7:A15" si="0">(A6+60000)</f>
         <v>220000</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="26">
         <v>33795.33</v>
       </c>
-      <c r="C7" s="30">
-        <v>0</v>
-      </c>
-      <c r="D7" s="30">
+      <c r="C7" s="27">
+        <v>0</v>
+      </c>
+      <c r="D7" s="27">
         <v>20236.330000000002</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="27">
         <v>16</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30">
+      <c r="F7" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="27">
         <v>31</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="29">
         <v>5.33</v>
       </c>
     </row>
@@ -4496,23 +4622,25 @@
         <f t="shared" si="0"/>
         <v>280000</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="26">
         <v>55115</v>
       </c>
-      <c r="C8" s="30">
-        <v>0</v>
-      </c>
-      <c r="D8" s="30">
+      <c r="C8" s="27">
+        <v>0</v>
+      </c>
+      <c r="D8" s="27">
         <v>32248</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="27">
         <v>15.33</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30">
+      <c r="F8" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="27">
         <v>41.67</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="29">
         <v>0</v>
       </c>
     </row>
@@ -4521,23 +4649,25 @@
         <f t="shared" si="0"/>
         <v>340000</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="26">
         <v>80971.67</v>
       </c>
-      <c r="C9" s="30">
-        <v>0</v>
-      </c>
-      <c r="D9" s="30">
+      <c r="C9" s="27">
+        <v>0</v>
+      </c>
+      <c r="D9" s="27">
         <v>48428.33</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="27">
         <v>31.33</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30">
+      <c r="F9" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="27">
         <v>41.67</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="29">
         <v>0</v>
       </c>
     </row>
@@ -4546,23 +4676,25 @@
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="26">
         <v>109939.67</v>
       </c>
-      <c r="C10" s="30">
-        <v>0</v>
-      </c>
-      <c r="D10" s="30">
+      <c r="C10" s="27">
+        <v>0</v>
+      </c>
+      <c r="D10" s="27">
         <v>66315.33</v>
       </c>
-      <c r="E10" s="30">
+      <c r="E10" s="27">
         <v>31</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30">
+      <c r="F10" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="27">
         <v>47</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="29">
         <v>0</v>
       </c>
     </row>
@@ -4571,23 +4703,25 @@
         <f t="shared" si="0"/>
         <v>460000</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="26">
         <v>147098</v>
       </c>
-      <c r="C11" s="30">
-        <v>0</v>
-      </c>
-      <c r="D11" s="30">
+      <c r="C11" s="27">
+        <v>0</v>
+      </c>
+      <c r="D11" s="27">
         <v>88567.33</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="27">
         <v>36.33</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30">
+      <c r="F11" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="27">
         <v>57</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="29">
         <v>0</v>
       </c>
     </row>
@@ -4596,23 +4730,25 @@
         <f t="shared" si="0"/>
         <v>520000</v>
       </c>
-      <c r="B12" s="29">
+      <c r="B12" s="26">
         <v>187221.33</v>
       </c>
-      <c r="C12" s="30">
-        <v>0</v>
-      </c>
-      <c r="D12" s="30">
+      <c r="C12" s="27">
+        <v>0</v>
+      </c>
+      <c r="D12" s="27">
         <v>112088.67</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="27">
         <v>36.67</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30">
+      <c r="F12" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="27">
         <v>62.33</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="29">
         <v>0</v>
       </c>
     </row>
@@ -4621,23 +4757,25 @@
         <f t="shared" si="0"/>
         <v>580000</v>
       </c>
-      <c r="B13" s="29">
+      <c r="B13" s="26">
         <v>229716</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="27">
         <v>5.33</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="27">
         <v>140063.32999999999</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="27">
         <v>36.33</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30">
+      <c r="F13" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="27">
         <v>67.67</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="29">
         <v>0</v>
       </c>
     </row>
@@ -4646,23 +4784,25 @@
         <f t="shared" si="0"/>
         <v>640000</v>
       </c>
-      <c r="B14" s="29">
+      <c r="B14" s="26">
         <v>279374</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="27">
         <v>5.33</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="27">
         <v>170454.67</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="27">
         <v>47</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30">
+      <c r="F14" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="27">
         <v>72.67</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="29">
         <v>10.33</v>
       </c>
     </row>
@@ -4671,23 +4811,25 @@
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="28">
         <v>334427.67</v>
       </c>
-      <c r="C15" s="33">
-        <v>0</v>
-      </c>
-      <c r="D15" s="33">
+      <c r="C15" s="30">
+        <v>0</v>
+      </c>
+      <c r="D15" s="30">
         <v>203676.67</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="30">
         <v>52</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33">
+      <c r="F15" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="30">
         <v>78</v>
       </c>
-      <c r="H15" s="34">
+      <c r="H15" s="31">
         <v>10.33</v>
       </c>
     </row>
@@ -4706,7 +4848,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H15"/>
+      <selection activeCell="F5" sqref="F5:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4715,26 +4857,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -4792,23 +4934,25 @@
       <c r="A5" s="6">
         <v>100000</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>6943</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>5.33</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>4114.33</v>
       </c>
-      <c r="E5" s="15">
-        <v>0</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15">
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="12">
         <v>10.33</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -4817,23 +4961,25 @@
         <f>(A5+60000)</f>
         <v>160000</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>18293.669999999998</v>
       </c>
-      <c r="C6" s="15">
-        <v>0</v>
-      </c>
-      <c r="D6" s="15">
+      <c r="C6" s="12">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
         <v>10589.67</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <v>10</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15">
+      <c r="F6" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="12">
         <v>20.67</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4842,23 +4988,25 @@
         <f t="shared" ref="A7:A15" si="0">(A6+60000)</f>
         <v>220000</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="11">
         <v>33925.33</v>
       </c>
-      <c r="C7" s="15">
-        <v>0</v>
-      </c>
-      <c r="D7" s="15">
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
         <v>20554.330000000002</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <v>15.67</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15">
+      <c r="F7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="12">
         <v>25.67</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="17">
         <v>5</v>
       </c>
     </row>
@@ -4867,23 +5015,25 @@
         <f t="shared" si="0"/>
         <v>280000</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>54927</v>
       </c>
-      <c r="C8" s="15">
-        <v>0</v>
-      </c>
-      <c r="D8" s="15">
+      <c r="C8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
         <v>32226.33</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <v>21</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15">
+      <c r="F8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="12">
         <v>42</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -4892,23 +5042,25 @@
         <f t="shared" si="0"/>
         <v>340000</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>81727.33</v>
       </c>
-      <c r="C9" s="15">
-        <v>0</v>
-      </c>
-      <c r="D9" s="15">
+      <c r="C9" s="12">
+        <v>0</v>
+      </c>
+      <c r="D9" s="12">
         <v>48432.67</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <v>20.67</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15">
+      <c r="F9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="12">
         <v>41.67</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -4917,23 +5069,25 @@
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="11">
         <v>110230.67</v>
       </c>
-      <c r="C10" s="15">
-        <v>0</v>
-      </c>
-      <c r="D10" s="15">
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+      <c r="D10" s="12">
         <v>66423.33</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <v>36.33</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15">
+      <c r="F10" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="12">
         <v>47</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -4942,23 +5096,25 @@
         <f t="shared" si="0"/>
         <v>460000</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>144234.32999999999</v>
       </c>
-      <c r="C11" s="15">
-        <v>0</v>
-      </c>
-      <c r="D11" s="15">
+      <c r="C11" s="12">
+        <v>0</v>
+      </c>
+      <c r="D11" s="12">
         <v>88348.67</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <v>36.33</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15">
+      <c r="F11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="12">
         <v>57.67</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="17">
         <v>0</v>
       </c>
     </row>
@@ -4967,23 +5123,25 @@
         <f t="shared" si="0"/>
         <v>520000</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="11">
         <v>184253.67</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>10.33</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>112455</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <v>41.67</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15">
+      <c r="F12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="12">
         <v>67.33</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -4992,23 +5150,25 @@
         <f t="shared" si="0"/>
         <v>580000</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>231609</v>
       </c>
-      <c r="C13" s="15">
-        <v>0</v>
-      </c>
-      <c r="D13" s="15">
+      <c r="C13" s="12">
+        <v>0</v>
+      </c>
+      <c r="D13" s="12">
         <v>140322.67000000001</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="12">
         <v>46.67</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15">
+      <c r="F13" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="12">
         <v>78</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5017,23 +5177,25 @@
         <f t="shared" si="0"/>
         <v>640000</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>279567</v>
       </c>
-      <c r="C14" s="15">
-        <v>0</v>
-      </c>
-      <c r="D14" s="15">
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12">
         <v>170804.67</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <v>52</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15">
+      <c r="F14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="12">
         <v>78</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -5042,23 +5204,25 @@
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="13">
         <v>333419</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="18">
         <v>5.33</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="18">
         <v>203917.67</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="18">
         <v>57.33</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21">
+      <c r="F15" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="18">
         <v>93.67</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="19">
         <v>5</v>
       </c>
     </row>
@@ -5076,7 +5240,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H15"/>
+      <selection activeCell="F5" sqref="F5:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5085,26 +5249,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -5162,23 +5326,25 @@
       <c r="A5" s="6">
         <v>100000</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>12277.33</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>2844</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>5594.33</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <v>5.33</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15">
+      <c r="F5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="12">
         <v>10.33</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -5187,23 +5353,25 @@
         <f>(A5+60000)</f>
         <v>160000</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>32576</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>7505.67</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>14574.33</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <v>10</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15">
+      <c r="F6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="12">
         <v>25.67</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5212,23 +5380,25 @@
         <f t="shared" ref="A7:A15" si="0">(A6+60000)</f>
         <v>220000</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="11">
         <v>60585.33</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>14142</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>27706</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <v>16</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15">
+      <c r="F7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="12">
         <v>26.33</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5237,23 +5407,25 @@
         <f t="shared" si="0"/>
         <v>280000</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>96863</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>23476.33</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>44316.33</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <v>21</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15">
+      <c r="F8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="12">
         <v>31</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5262,23 +5434,25 @@
         <f t="shared" si="0"/>
         <v>340000</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>144229.67000000001</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>34310.67</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>64914.67</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <v>26</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15">
+      <c r="F9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="12">
         <v>41.33</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5287,23 +5461,25 @@
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="11">
         <v>199129.33</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>47526.33</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>90814.67</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <v>15.67</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15">
+      <c r="F10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="12">
         <v>46.67</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -5312,23 +5488,25 @@
         <f t="shared" si="0"/>
         <v>460000</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>262138.33</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>63283</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>120128.33</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <v>36.67</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15">
+      <c r="F11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="12">
         <v>52</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="17">
         <v>5</v>
       </c>
     </row>
@@ -5337,23 +5515,25 @@
         <f t="shared" si="0"/>
         <v>520000</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="11">
         <v>338122</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>81138.67</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>152823</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <v>36.67</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15">
+      <c r="F12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="12">
         <v>62</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -5362,23 +5542,25 @@
         <f t="shared" si="0"/>
         <v>580000</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>419936.67</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>101760.33</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>188596.33</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="12">
         <v>36.33</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15">
+      <c r="F13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="12">
         <v>73</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5387,23 +5569,25 @@
         <f t="shared" si="0"/>
         <v>640000</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>502973.67</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>123199.67</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>228362.67</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <v>41.67</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15">
+      <c r="F14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="12">
         <v>78</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5412,23 +5596,25 @@
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="13">
         <v>610071.67000000004</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="18">
         <v>147108.67000000001</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="18">
         <v>271704.67</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="18">
         <v>46.67</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21">
+      <c r="F15" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="18">
         <v>88.67</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="19">
         <v>5.33</v>
       </c>
     </row>
@@ -5455,26 +5641,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -5532,23 +5718,23 @@
       <c r="A5" s="6">
         <v>100000</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="11">
         <v>12470.33</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>2839</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="12">
         <v>16679</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="12">
         <v>5.33</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15">
+      <c r="F5" s="12"/>
+      <c r="G5" s="12">
         <v>20.329999999999998</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5557,23 +5743,23 @@
         <f>(A5+60000)</f>
         <v>160000</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>31029.67</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>7501</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="12">
         <v>46230</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="12">
         <v>10.67</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12">
         <v>15.33</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5582,23 +5768,23 @@
         <f t="shared" ref="A7:A15" si="0">(A6+60000)</f>
         <v>220000</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="11">
         <v>60023.33</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>14147.33</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="12">
         <v>81571.33</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="12">
         <v>15.67</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12">
         <v>31.67</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5607,23 +5793,23 @@
         <f t="shared" si="0"/>
         <v>280000</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>101923.33</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>23513</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="12">
         <v>120288.33</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
         <v>21</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15">
+      <c r="F8" s="12"/>
+      <c r="G8" s="12">
         <v>36.33</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5632,23 +5818,23 @@
         <f t="shared" si="0"/>
         <v>340000</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="11">
         <v>150274</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>34431.67</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="12">
         <v>160780</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="12">
         <v>26.33</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15">
+      <c r="F9" s="12"/>
+      <c r="G9" s="12">
         <v>51.67</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5657,23 +5843,23 @@
         <f t="shared" si="0"/>
         <v>400000</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="11">
         <v>198567</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>47452.33</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="12">
         <v>204434</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="12">
         <v>25.67</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12">
         <v>47</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="17">
         <v>0</v>
       </c>
     </row>
@@ -5682,23 +5868,23 @@
         <f t="shared" si="0"/>
         <v>460000</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="11">
         <v>263865.33</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>63198.67</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="12">
         <v>249000.67</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="12">
         <v>31.33</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15">
+      <c r="F11" s="12"/>
+      <c r="G11" s="12">
         <v>52.33</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="17">
         <v>10.33</v>
       </c>
     </row>
@@ -5707,23 +5893,23 @@
         <f t="shared" si="0"/>
         <v>520000</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="11">
         <v>341493.33</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>80550</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="12">
         <v>295198</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="12">
         <v>31.33</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15">
+      <c r="F12" s="12"/>
+      <c r="G12" s="12">
         <v>57.33</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="17">
         <v>10.33</v>
       </c>
     </row>
@@ -5732,23 +5918,23 @@
         <f t="shared" si="0"/>
         <v>580000</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="11">
         <v>415190.33</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>100838</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="12">
         <v>343810.33</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="12">
         <v>47</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15">
+      <c r="F13" s="12"/>
+      <c r="G13" s="12">
         <v>72.67</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="17">
         <v>5.33</v>
       </c>
     </row>
@@ -5757,23 +5943,23 @@
         <f t="shared" si="0"/>
         <v>640000</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="11">
         <v>502986.67</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>122389</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="12">
         <v>395997</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="12">
         <v>41.67</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15">
+      <c r="F14" s="12"/>
+      <c r="G14" s="12">
         <v>83.33</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="17">
         <v>5</v>
       </c>
     </row>
@@ -5782,23 +5968,23 @@
         <f t="shared" si="0"/>
         <v>700000</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="13">
         <v>604516</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="18">
         <v>147876.32999999999</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="18">
         <v>449098</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="18">
         <v>47</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21">
+      <c r="F15" s="18"/>
+      <c r="G15" s="18">
         <v>88.67</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="19">
         <v>5.33</v>
       </c>
     </row>

</xml_diff>